<commit_message>
Bug fixes (CDCM statistics).
</commit_message>
<xml_diff>
--- a/other/Handmade/StatsCDCM.xlsx
+++ b/other/Handmade/StatsCDCM.xlsx
@@ -10,7 +10,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$4:$H$15</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$4:$H$14</definedName>
   </definedNames>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="27">
   <si>
     <t>Capacity (kVA)</t>
   </si>
@@ -63,9 +63,6 @@
     <t>^(?:|LDNO .*: |Margin.*: )LV.*HH Metered$</t>
   </si>
   <si>
-    <t>^LV.*HH Metered$</t>
-  </si>
-  <si>
     <t>^(?:LV|LV Sub|HV|LDNO .*) HH Metered$</t>
   </si>
   <si>
@@ -90,22 +87,22 @@
     <t>Customer F</t>
   </si>
   <si>
-    <t>Customer G</t>
-  </si>
-  <si>
-    <t>Customer H</t>
-  </si>
-  <si>
-    <t>Customer I</t>
-  </si>
-  <si>
-    <t>Customer J</t>
-  </si>
-  <si>
-    <t>Customer K</t>
-  </si>
-  <si>
-    <t>Customer L</t>
+    <t>500kVA continuous</t>
+  </si>
+  <si>
+    <t>500kVA off-peak</t>
+  </si>
+  <si>
+    <t>5MVA continuous</t>
+  </si>
+  <si>
+    <t>5MVA off-peak</t>
+  </si>
+  <si>
+    <t>500kVA peaky</t>
+  </si>
+  <si>
+    <t>5MVA peaky</t>
   </si>
 </sst>
 </file>
@@ -195,9 +192,23 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="118">
+  <cellStyleXfs count="132">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -346,7 +357,7 @@
       <protection locked="0"/>
     </xf>
   </cellXfs>
-  <cellStyles count="118">
+  <cellStyles count="132">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
@@ -406,6 +417,13 @@
     <cellStyle name="Followed Hyperlink" xfId="113" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="115" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="117" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="119" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="121" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="123" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="125" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="127" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="129" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="131" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
@@ -464,6 +482,13 @@
     <cellStyle name="Hyperlink" xfId="112" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="114" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="116" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="118" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="120" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="122" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="124" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="126" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="128" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="130" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -811,24 +836,6 @@
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="4">
-        <v>0</v>
-      </c>
-      <c r="D2" s="4">
-        <v>1</v>
-      </c>
-      <c r="E2" s="4">
-        <v>2</v>
-      </c>
-      <c r="F2" s="4">
-        <v>3</v>
-      </c>
-      <c r="G2" s="4">
-        <v>4</v>
-      </c>
-      <c r="H2" s="4">
-        <v>5</v>
-      </c>
     </row>
     <row r="4" spans="1:8" ht="28">
       <c r="B4" s="2" t="s">
@@ -855,7 +862,7 @@
     </row>
     <row r="5" spans="1:8">
       <c r="A5" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B5" s="8" t="s">
         <v>8</v>
@@ -875,7 +882,7 @@
     </row>
     <row r="6" spans="1:8">
       <c r="A6" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B6" s="8" t="s">
         <v>8</v>
@@ -895,7 +902,7 @@
     </row>
     <row r="7" spans="1:8">
       <c r="A7" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B7" s="8" t="s">
         <v>9</v>
@@ -921,7 +928,7 @@
     </row>
     <row r="8" spans="1:8">
       <c r="A8" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B8" s="8" t="s">
         <v>10</v>
@@ -947,7 +954,7 @@
     </row>
     <row r="9" spans="1:8">
       <c r="A9" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B9" s="8" t="s">
         <v>11</v>
@@ -965,139 +972,139 @@
     </row>
     <row r="10" spans="1:8">
       <c r="A10" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B10" s="8" t="s">
         <v>12</v>
       </c>
       <c r="C10" s="5">
-        <v>55</v>
-      </c>
-      <c r="D10" s="5"/>
+        <v>35</v>
+      </c>
+      <c r="D10" s="5">
+        <v>48</v>
+      </c>
       <c r="E10" s="6">
-        <v>200</v>
-      </c>
-      <c r="F10" s="6"/>
-      <c r="G10" s="6"/>
+        <v>140</v>
+      </c>
+      <c r="F10" s="6">
+        <v>160</v>
+      </c>
+      <c r="G10" s="6">
+        <v>32.5</v>
+      </c>
       <c r="H10" s="7">
-        <v>250</v>
+        <v>500</v>
       </c>
     </row>
     <row r="11" spans="1:8">
       <c r="A11" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B11" s="8" t="s">
         <v>13</v>
       </c>
       <c r="C11" s="5"/>
-      <c r="D11" s="5">
-        <v>77</v>
-      </c>
+      <c r="D11" s="5"/>
       <c r="E11" s="6"/>
-      <c r="F11" s="6">
-        <v>200</v>
-      </c>
-      <c r="G11" s="6"/>
+      <c r="F11" s="6"/>
+      <c r="G11" s="6">
+        <v>450</v>
+      </c>
       <c r="H11" s="7">
-        <v>250</v>
+        <v>500</v>
       </c>
     </row>
     <row r="12" spans="1:8">
       <c r="A12" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="C12" s="5">
-        <v>35</v>
-      </c>
+        <v>13</v>
+      </c>
+      <c r="C12" s="5"/>
       <c r="D12" s="5">
-        <v>100</v>
-      </c>
-      <c r="E12" s="6">
-        <v>400</v>
-      </c>
+        <v>77</v>
+      </c>
+      <c r="E12" s="6"/>
       <c r="F12" s="6">
-        <v>100</v>
-      </c>
-      <c r="G12" s="6">
-        <v>300</v>
-      </c>
+        <v>450</v>
+      </c>
+      <c r="G12" s="6"/>
       <c r="H12" s="7">
         <v>500</v>
       </c>
     </row>
     <row r="13" spans="1:8">
       <c r="A13" s="3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="C13" s="5"/>
+        <v>13</v>
+      </c>
+      <c r="C13" s="5">
+        <v>55</v>
+      </c>
       <c r="D13" s="5"/>
-      <c r="E13" s="6"/>
+      <c r="E13" s="6">
+        <v>250</v>
+      </c>
       <c r="F13" s="6"/>
-      <c r="G13" s="6">
-        <v>450</v>
-      </c>
+      <c r="G13" s="6"/>
       <c r="H13" s="7">
         <v>500</v>
       </c>
     </row>
     <row r="14" spans="1:8">
       <c r="A14" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C14" s="5"/>
-      <c r="D14" s="5">
-        <v>77</v>
-      </c>
+      <c r="D14" s="5"/>
       <c r="E14" s="6"/>
-      <c r="F14" s="6">
+      <c r="F14" s="6"/>
+      <c r="G14" s="6">
         <v>4500</v>
       </c>
-      <c r="G14" s="6"/>
       <c r="H14" s="7">
         <v>5000</v>
       </c>
     </row>
     <row r="15" spans="1:8">
       <c r="A15" s="3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C15" s="5"/>
-      <c r="D15" s="5"/>
+      <c r="D15" s="5">
+        <v>77</v>
+      </c>
       <c r="E15" s="6"/>
-      <c r="F15" s="6"/>
-      <c r="G15" s="6">
+      <c r="F15" s="6">
         <v>4500</v>
       </c>
+      <c r="G15" s="6"/>
       <c r="H15" s="7">
         <v>5000</v>
       </c>
     </row>
     <row r="16" spans="1:8">
       <c r="A16" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C16" s="5">
         <v>55</v>
       </c>
       <c r="D16" s="5"/>
       <c r="E16" s="6">
-        <v>4500</v>
+        <v>250</v>
       </c>
       <c r="F16" s="6"/>
       <c r="G16" s="6"/>

</xml_diff>

<commit_message>
Improvements to data management and statistics tools.
</commit_message>
<xml_diff>
--- a/other/Handmade/StatsCDCM.xlsx
+++ b/other/Handmade/StatsCDCM.xlsx
@@ -10,7 +10,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$4:$H$14</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$4:$K$21</definedName>
   </definedNames>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="36">
   <si>
     <t>Capacity (kVA)</t>
   </si>
@@ -51,71 +51,106 @@
     <t>^(?:|LDNO .*: |Margin.*: )(?:Domestic Unrestricted|LV Network Dom)</t>
   </si>
   <si>
-    <t>^(?:(Small Non )?Domestic (?:Unrestricted|Two)|LV.*Medium|LV Network)</t>
-  </si>
-  <si>
     <t>^(?:|LDNO .*: |Margin.*: )(?:Small Non Domestic (?:Unrestricted|Two)|LV.*(?:HH Metered$|Medium)|LV Network)</t>
   </si>
   <si>
     <t>^(?:Small Non Domestic (?:Unrestricted|Two)|LV.*(?:HH Metered$|Medium)|LV Network)</t>
   </si>
   <si>
-    <t>^(?:|LDNO .*: |Margin.*: )LV.*HH Metered$</t>
-  </si>
-  <si>
     <t>^(?:LV|LV Sub|HV|LDNO .*) HH Metered$</t>
   </si>
   <si>
     <t>^HV HH Metered$</t>
   </si>
   <si>
-    <t>Customer A</t>
-  </si>
-  <si>
-    <t>Customer B</t>
-  </si>
-  <si>
-    <t>Customer C</t>
-  </si>
-  <si>
-    <t>Customer D</t>
-  </si>
-  <si>
-    <t>Customer E</t>
-  </si>
-  <si>
-    <t>Customer F</t>
+    <t>Total kWh/year</t>
+  </si>
+  <si>
+    <t>Rate 2 kWh/year</t>
+  </si>
+  <si>
+    <t>Load factor (kW/kVA)</t>
+  </si>
+  <si>
+    <t>^(?:|LDNO .*: |Margin.*: )(?:Domestic (?:Unrestricted|Two)|LV Network Dom)</t>
+  </si>
+  <si>
+    <t>Average home</t>
+  </si>
+  <si>
+    <t>Average home x250</t>
+  </si>
+  <si>
+    <t>Average home x2500</t>
+  </si>
+  <si>
+    <t>Electric heating home</t>
+  </si>
+  <si>
+    <t>Electric heating home x100</t>
+  </si>
+  <si>
+    <t>Electric heating home x1000</t>
+  </si>
+  <si>
+    <t>Low use home</t>
   </si>
   <si>
     <t>500kVA continuous</t>
   </si>
   <si>
+    <t>5MVA continuous</t>
+  </si>
+  <si>
+    <t>68kVA continuous</t>
+  </si>
+  <si>
+    <t>500kVA business</t>
+  </si>
+  <si>
     <t>500kVA off-peak</t>
   </si>
   <si>
-    <t>5MVA continuous</t>
+    <t>500kVA random</t>
   </si>
   <si>
     <t>5MVA off-peak</t>
   </si>
   <si>
-    <t>500kVA peaky</t>
-  </si>
-  <si>
-    <t>5MVA peaky</t>
+    <t>5MVA random</t>
+  </si>
+  <si>
+    <t>68kVA business</t>
+  </si>
+  <si>
+    <t>68kVA off-peak</t>
+  </si>
+  <si>
+    <t>68kVA random</t>
+  </si>
+  <si>
+    <t>5MVA business</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="4">
+  <numFmts count="5">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="\ _(???,???,??0_);[Red]\ \(???,???,??0\);;@"/>
     <numFmt numFmtId="165" formatCode="_-* #,##0.0_-;\-* #,##0.0_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="166" formatCode="_-* #,##0.000_-;\-* #,##0.000_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="167" formatCode="??0.0%"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -163,7 +198,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -182,6 +217,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -192,149 +233,234 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="132">
+  <cellStyleXfs count="217">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -356,8 +482,14 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="4" borderId="0" xfId="132" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="132">
+  <cellStyles count="217">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
@@ -424,6 +556,48 @@
     <cellStyle name="Followed Hyperlink" xfId="127" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="129" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="131" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="134" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="136" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="138" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="140" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="142" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="144" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="146" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="148" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="150" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="152" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="154" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="156" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="158" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="160" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="162" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="164" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="166" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="168" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="170" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="172" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="174" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="176" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="178" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="180" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="182" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="184" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="186" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="188" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="190" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="192" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="194" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="196" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="198" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="200" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="202" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="204" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="206" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="208" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="210" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="212" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="214" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="216" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
@@ -489,7 +663,50 @@
     <cellStyle name="Hyperlink" xfId="126" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="128" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="130" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="133" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="135" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="137" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="139" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="141" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="143" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="145" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="147" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="149" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="151" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="153" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="155" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="157" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="159" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="161" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="163" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="165" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="167" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="169" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="171" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="173" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="175" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="177" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="179" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="181" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="183" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="185" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="187" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="189" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="191" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="193" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="195" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="197" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="199" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="201" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="203" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="205" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="207" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="209" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="211" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="213" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="215" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="132" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
@@ -818,26 +1035,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:H16"/>
+  <dimension ref="A2:K23"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.1640625" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="22" style="4" customWidth="1"/>
-    <col min="2" max="2" width="97" style="4" customWidth="1"/>
+    <col min="1" max="1" width="29.33203125" style="4" customWidth="1"/>
+    <col min="2" max="2" width="59.33203125" style="4" customWidth="1"/>
     <col min="3" max="8" width="13.83203125" style="4" customWidth="1"/>
     <col min="9" max="16384" width="14.1640625" style="4"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:8" ht="19">
+    <row r="2" spans="1:11" ht="19">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="28">
+    <row r="4" spans="1:11" ht="28">
       <c r="B4" s="2" t="s">
         <v>7</v>
       </c>
@@ -859,260 +1076,711 @@
       <c r="H4" s="2" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:8">
+      <c r="I4" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="34" customHeight="1">
       <c r="A5" s="3" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="C5" s="5">
-        <v>35</v>
-      </c>
-      <c r="D5" s="5"/>
+        <v>66</v>
+      </c>
+      <c r="D5" s="5">
+        <v>77</v>
+      </c>
       <c r="E5" s="6">
-        <v>0.41649999999999998</v>
-      </c>
-      <c r="F5" s="6"/>
+        <f>0.71*H5</f>
+        <v>355</v>
+      </c>
+      <c r="F5" s="6">
+        <f>0.2*H5</f>
+        <v>100</v>
+      </c>
       <c r="G5" s="6">
-        <v>0.15</v>
-      </c>
-      <c r="H5" s="7"/>
-    </row>
-    <row r="6" spans="1:8">
+        <f>0.2*H5</f>
+        <v>100</v>
+      </c>
+      <c r="H5" s="7">
+        <v>500</v>
+      </c>
+      <c r="I5" s="9">
+        <f>(C5*E5+D5*F5+(168-C5-D5)*G5)*365/7</f>
+        <v>1753564.2857142857</v>
+      </c>
+      <c r="J5" s="9">
+        <f>D5*F5*365/7</f>
+        <v>401500</v>
+      </c>
+      <c r="K5" s="10">
+        <f>I5/365/24/H5</f>
+        <v>0.40035714285714286</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="34" customHeight="1">
       <c r="A6" s="3" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6" s="5">
-        <v>35</v>
-      </c>
+        <v>11</v>
+      </c>
+      <c r="C6" s="5"/>
       <c r="D6" s="5"/>
-      <c r="E6" s="6">
-        <v>0.83250000000000002</v>
-      </c>
+      <c r="E6" s="6"/>
       <c r="F6" s="6"/>
       <c r="G6" s="6">
-        <v>0.3</v>
-      </c>
-      <c r="H6" s="7"/>
-    </row>
-    <row r="7" spans="1:8">
+        <f>0.9*H6</f>
+        <v>450</v>
+      </c>
+      <c r="H6" s="7">
+        <v>500</v>
+      </c>
+      <c r="I6" s="9">
+        <f>(C6*E6+D6*F6+(168-C6-D6)*G6)*365/7</f>
+        <v>3942000</v>
+      </c>
+      <c r="J6" s="9">
+        <f>D6*F6*365/7</f>
+        <v>0</v>
+      </c>
+      <c r="K6" s="10">
+        <f>I6/365/24/H6</f>
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="34" customHeight="1">
       <c r="A7" s="3" t="s">
-        <v>17</v>
+        <v>28</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="C7" s="5">
+        <v>11</v>
+      </c>
+      <c r="C7" s="5"/>
+      <c r="D7" s="5">
+        <f>0.4*168/0.9</f>
+        <v>74.666666666666671</v>
+      </c>
+      <c r="E7" s="6"/>
+      <c r="F7" s="6">
+        <f>0.9*H7</f>
+        <v>450</v>
+      </c>
+      <c r="G7" s="6"/>
+      <c r="H7" s="7">
+        <v>500</v>
+      </c>
+      <c r="I7" s="9">
+        <f>(C7*E7+D7*F7+(168-C7-D7)*G7)*365/7</f>
+        <v>1752000</v>
+      </c>
+      <c r="J7" s="9">
+        <f>D7*F7*365/7</f>
+        <v>1752000</v>
+      </c>
+      <c r="K7" s="10">
+        <f>I7/365/24/H7</f>
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="34" customHeight="1">
+      <c r="A8" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" s="5"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="6"/>
+      <c r="G8" s="6">
+        <f>0.4*H8</f>
+        <v>200</v>
+      </c>
+      <c r="H8" s="7">
+        <v>500</v>
+      </c>
+      <c r="I8" s="9">
+        <f>(C8*E8+D8*F8+(168-C8-D8)*G8)*365/7</f>
+        <v>1752000</v>
+      </c>
+      <c r="J8" s="9">
+        <f>D8*F8*365/7</f>
+        <v>0</v>
+      </c>
+      <c r="K8" s="10">
+        <f>I8/365/24/H8</f>
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="34" customHeight="1">
+      <c r="A9" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="D7" s="5">
-        <v>48</v>
-      </c>
-      <c r="E7" s="6">
-        <v>0.75</v>
-      </c>
-      <c r="F7" s="6">
-        <v>0.99950000000000006</v>
-      </c>
-      <c r="G7" s="6">
-        <v>0.3</v>
-      </c>
-      <c r="H7" s="7">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8">
-      <c r="A8" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B8" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="C8" s="5">
-        <v>35</v>
-      </c>
-      <c r="D8" s="5">
-        <v>100</v>
-      </c>
-      <c r="E8" s="6">
-        <v>60</v>
-      </c>
-      <c r="F8" s="6">
-        <v>1</v>
-      </c>
-      <c r="G8" s="6">
-        <v>50</v>
-      </c>
-      <c r="H8" s="7">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8">
-      <c r="A9" s="3" t="s">
-        <v>19</v>
-      </c>
       <c r="B9" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="C9" s="5"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="6"/>
-      <c r="F9" s="6"/>
+        <v>12</v>
+      </c>
+      <c r="C9" s="5">
+        <v>66</v>
+      </c>
+      <c r="D9" s="5">
+        <v>77</v>
+      </c>
+      <c r="E9" s="6">
+        <f>0.71*H9</f>
+        <v>3550</v>
+      </c>
+      <c r="F9" s="6">
+        <f>0.2*H9</f>
+        <v>1000</v>
+      </c>
       <c r="G9" s="6">
-        <v>65</v>
+        <f>0.2*H9</f>
+        <v>1000</v>
       </c>
       <c r="H9" s="7">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8">
+        <v>5000</v>
+      </c>
+      <c r="I9" s="9">
+        <f>(C9*E9+D9*F9+(168-C9-D9)*G9)*365/7</f>
+        <v>17535642.857142858</v>
+      </c>
+      <c r="J9" s="9">
+        <f>D9*F9*365/7</f>
+        <v>4015000</v>
+      </c>
+      <c r="K9" s="10">
+        <f>I9/365/24/H9</f>
+        <v>0.40035714285714291</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="34" customHeight="1">
       <c r="A10" s="3" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="B10" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="C10" s="5">
-        <v>35</v>
-      </c>
-      <c r="D10" s="5">
-        <v>48</v>
-      </c>
-      <c r="E10" s="6">
-        <v>140</v>
-      </c>
-      <c r="F10" s="6">
-        <v>160</v>
-      </c>
+      <c r="C10" s="5"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="6"/>
       <c r="G10" s="6">
-        <v>32.5</v>
+        <f>0.9*H10</f>
+        <v>4500</v>
       </c>
       <c r="H10" s="7">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8">
+        <v>5000</v>
+      </c>
+      <c r="I10" s="9">
+        <f>(C10*E10+D10*F10+(168-C10-D10)*G10)*365/7</f>
+        <v>39420000</v>
+      </c>
+      <c r="J10" s="9">
+        <f>D10*F10*365/7</f>
+        <v>0</v>
+      </c>
+      <c r="K10" s="10">
+        <f>I10/365/24/H10</f>
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" ht="34" customHeight="1">
       <c r="A11" s="3" t="s">
-        <v>21</v>
+        <v>30</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C11" s="5"/>
-      <c r="D11" s="5"/>
+      <c r="D11" s="5">
+        <f>0.4*168/0.9</f>
+        <v>74.666666666666671</v>
+      </c>
       <c r="E11" s="6"/>
-      <c r="F11" s="6"/>
-      <c r="G11" s="6">
-        <v>450</v>
-      </c>
+      <c r="F11" s="6">
+        <f>0.9*H11</f>
+        <v>4500</v>
+      </c>
+      <c r="G11" s="6"/>
       <c r="H11" s="7">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8">
+        <v>5000</v>
+      </c>
+      <c r="I11" s="9">
+        <f>(C11*E11+D11*F11+(168-C11-D11)*G11)*365/7</f>
+        <v>17520000</v>
+      </c>
+      <c r="J11" s="9">
+        <f>D11*F11*365/7</f>
+        <v>17520000</v>
+      </c>
+      <c r="K11" s="10">
+        <f>I11/365/24/H11</f>
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" ht="34" customHeight="1">
       <c r="A12" s="3" t="s">
-        <v>22</v>
+        <v>31</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C12" s="5"/>
-      <c r="D12" s="5">
+      <c r="D12" s="5"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="6"/>
+      <c r="G12" s="6">
+        <f>0.4*H12</f>
+        <v>2000</v>
+      </c>
+      <c r="H12" s="7">
+        <v>5000</v>
+      </c>
+      <c r="I12" s="9">
+        <f>(C12*E12+D12*F12+(168-C12-D12)*G12)*365/7</f>
+        <v>17520000</v>
+      </c>
+      <c r="J12" s="9">
+        <f>D12*F12*365/7</f>
+        <v>0</v>
+      </c>
+      <c r="K12" s="10">
+        <f>I12/365/24/H12</f>
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" ht="34" customHeight="1">
+      <c r="A13" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B13" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C13" s="5">
+        <v>66</v>
+      </c>
+      <c r="D13" s="5">
         <v>77</v>
       </c>
-      <c r="E12" s="6"/>
-      <c r="F12" s="6">
-        <v>450</v>
-      </c>
-      <c r="G12" s="6"/>
-      <c r="H12" s="7">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8">
-      <c r="A13" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="B13" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="C13" s="5">
-        <v>55</v>
-      </c>
-      <c r="D13" s="5"/>
       <c r="E13" s="6">
-        <v>250</v>
-      </c>
-      <c r="F13" s="6"/>
-      <c r="G13" s="6"/>
+        <f>0.71*H13</f>
+        <v>48.28</v>
+      </c>
+      <c r="F13" s="6">
+        <f>0.2*H13</f>
+        <v>13.600000000000001</v>
+      </c>
+      <c r="G13" s="6">
+        <f>0.2*H13</f>
+        <v>13.600000000000001</v>
+      </c>
       <c r="H13" s="7">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8">
+        <v>68</v>
+      </c>
+      <c r="I13" s="9">
+        <f>(C13*E13+D13*F13+(168-C13-D13)*G13)*365/7</f>
+        <v>238484.74285714288</v>
+      </c>
+      <c r="J13" s="9">
+        <f>D13*F13*365/7</f>
+        <v>54604</v>
+      </c>
+      <c r="K13" s="10">
+        <f>I13/365/24/H13</f>
+        <v>0.40035714285714291</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" ht="34" customHeight="1">
       <c r="A14" s="3" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C14" s="5"/>
       <c r="D14" s="5"/>
       <c r="E14" s="6"/>
       <c r="F14" s="6"/>
       <c r="G14" s="6">
-        <v>4500</v>
+        <f>0.9*H14</f>
+        <v>61.2</v>
       </c>
       <c r="H14" s="7">
-        <v>5000</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8">
+        <v>68</v>
+      </c>
+      <c r="I14" s="9">
+        <f>(C14*E14+D14*F14+(168-C14-D14)*G14)*365/7</f>
+        <v>536112</v>
+      </c>
+      <c r="J14" s="9">
+        <f>D14*F14*365/7</f>
+        <v>0</v>
+      </c>
+      <c r="K14" s="10">
+        <f>I14/365/24/H14</f>
+        <v>0.89999999999999991</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" ht="34" customHeight="1">
       <c r="A15" s="3" t="s">
-        <v>24</v>
+        <v>33</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C15" s="5"/>
       <c r="D15" s="5">
-        <v>77</v>
+        <f>0.4*168/0.9</f>
+        <v>74.666666666666671</v>
       </c>
       <c r="E15" s="6"/>
       <c r="F15" s="6">
-        <v>4500</v>
+        <f>0.9*H15</f>
+        <v>61.2</v>
       </c>
       <c r="G15" s="6"/>
       <c r="H15" s="7">
+        <v>68</v>
+      </c>
+      <c r="I15" s="9">
+        <f>(C15*E15+D15*F15+(168-C15-D15)*G15)*365/7</f>
+        <v>238272.00000000003</v>
+      </c>
+      <c r="J15" s="9">
+        <f>D15*F15*365/7</f>
+        <v>238272.00000000003</v>
+      </c>
+      <c r="K15" s="10">
+        <f>I15/365/24/H15</f>
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" ht="34" customHeight="1">
+      <c r="A16" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B16" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="C16" s="5"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="6"/>
+      <c r="F16" s="6"/>
+      <c r="G16" s="6">
+        <f>0.4*H16</f>
+        <v>27.200000000000003</v>
+      </c>
+      <c r="H16" s="7">
+        <v>68</v>
+      </c>
+      <c r="I16" s="9">
+        <f>(C16*E16+D16*F16+(168-C16-D16)*G16)*365/7</f>
+        <v>238272.00000000003</v>
+      </c>
+      <c r="J16" s="9">
+        <f>D16*F16*365/7</f>
+        <v>0</v>
+      </c>
+      <c r="K16" s="10">
+        <f>I16/365/24/H16</f>
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" ht="34" customHeight="1">
+      <c r="A17" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B17" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C17" s="5">
+        <v>35</v>
+      </c>
+      <c r="D17" s="5">
+        <v>49</v>
+      </c>
+      <c r="E17" s="6">
+        <v>1</v>
+      </c>
+      <c r="F17" s="6">
+        <v>0.1</v>
+      </c>
+      <c r="G17" s="6">
+        <v>0.4</v>
+      </c>
+      <c r="H17" s="7">
+        <v>6</v>
+      </c>
+      <c r="I17" s="9">
+        <f>(C17*E17+D17*F17+(168-C17-D17)*G17)*365/7</f>
+        <v>3832.5</v>
+      </c>
+      <c r="J17" s="9">
+        <f>D17*F17*365/7</f>
+        <v>255.50000000000003</v>
+      </c>
+      <c r="K17" s="10">
+        <f>I17/365/24/H17</f>
+        <v>7.2916666666666671E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" ht="34" customHeight="1">
+      <c r="A18" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B18" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C18" s="5">
+        <v>35</v>
+      </c>
+      <c r="D18" s="5">
+        <v>49</v>
+      </c>
+      <c r="E18" s="6">
+        <f>H18/2</f>
+        <v>250</v>
+      </c>
+      <c r="F18" s="6">
+        <f>H18/20</f>
+        <v>25</v>
+      </c>
+      <c r="G18" s="6">
+        <f>H18/5</f>
+        <v>100</v>
+      </c>
+      <c r="H18" s="7">
+        <v>500</v>
+      </c>
+      <c r="I18" s="9">
+        <f>(C18*E18+D18*F18+(168-C18-D18)*G18)*365/7</f>
+        <v>958125</v>
+      </c>
+      <c r="J18" s="9">
+        <f>D18*F18*365/7</f>
+        <v>63875</v>
+      </c>
+      <c r="K18" s="10">
+        <f>I18/365/24/H18</f>
+        <v>0.21875</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" ht="34" customHeight="1">
+      <c r="A19" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B19" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C19" s="5">
+        <v>35</v>
+      </c>
+      <c r="D19" s="5">
+        <v>49</v>
+      </c>
+      <c r="E19" s="6">
+        <f>H19/2</f>
+        <v>2500</v>
+      </c>
+      <c r="F19" s="6">
+        <f>H19/20</f>
+        <v>250</v>
+      </c>
+      <c r="G19" s="6">
+        <f>H19/5</f>
+        <v>1000</v>
+      </c>
+      <c r="H19" s="7">
         <v>5000</v>
       </c>
-    </row>
-    <row r="16" spans="1:8">
-      <c r="A16" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="B16" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="C16" s="5">
-        <v>55</v>
-      </c>
-      <c r="D16" s="5"/>
-      <c r="E16" s="6">
-        <v>250</v>
-      </c>
-      <c r="F16" s="6"/>
-      <c r="G16" s="6"/>
-      <c r="H16" s="7">
+      <c r="I19" s="9">
+        <f>(C19*E19+D19*F19+(168-C19-D19)*G19)*365/7</f>
+        <v>9581250</v>
+      </c>
+      <c r="J19" s="9">
+        <f>D19*F19*365/7</f>
+        <v>638750</v>
+      </c>
+      <c r="K19" s="10">
+        <f>I19/365/24/H19</f>
+        <v>0.21875</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" ht="34" customHeight="1">
+      <c r="A20" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B20" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C20" s="5">
+        <v>35</v>
+      </c>
+      <c r="D20" s="5">
+        <v>49</v>
+      </c>
+      <c r="E20" s="6">
+        <v>1.25</v>
+      </c>
+      <c r="F20" s="6">
+        <v>1.5</v>
+      </c>
+      <c r="G20" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="H20" s="7">
+        <v>18</v>
+      </c>
+      <c r="I20" s="9">
+        <f>(C20*E20+D20*F20+(168-C20-D20)*G20)*365/7</f>
+        <v>8303.75</v>
+      </c>
+      <c r="J20" s="9">
+        <f>D20*F20*365/7</f>
+        <v>3832.5</v>
+      </c>
+      <c r="K20" s="10">
+        <f>I20/365/24/H20</f>
+        <v>5.2662037037037035E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" ht="34" customHeight="1">
+      <c r="A21" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B21" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C21" s="5">
+        <v>35</v>
+      </c>
+      <c r="D21" s="5">
+        <v>49</v>
+      </c>
+      <c r="E21" s="6">
+        <f>1.25*H21/5</f>
+        <v>125</v>
+      </c>
+      <c r="F21" s="6">
+        <f>1.5*H21/5</f>
+        <v>150</v>
+      </c>
+      <c r="G21" s="6">
+        <f>0.5*H21/5</f>
+        <v>50</v>
+      </c>
+      <c r="H21" s="7">
+        <v>500</v>
+      </c>
+      <c r="I21" s="9">
+        <f>(C21*E21+D21*F21+(168-C21-D21)*G21)*365/7</f>
+        <v>830375</v>
+      </c>
+      <c r="J21" s="9">
+        <f>D21*F21*365/7</f>
+        <v>383250</v>
+      </c>
+      <c r="K21" s="10">
+        <f>I21/365/24/H21</f>
+        <v>0.18958333333333335</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" ht="34" customHeight="1">
+      <c r="A22" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B22" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C22" s="5">
+        <v>35</v>
+      </c>
+      <c r="D22" s="5">
+        <v>49</v>
+      </c>
+      <c r="E22" s="6">
+        <f>1.25*H22/5</f>
+        <v>1250</v>
+      </c>
+      <c r="F22" s="6">
+        <f>1.5*H22/5</f>
+        <v>1500</v>
+      </c>
+      <c r="G22" s="6">
+        <f>0.5*H22/5</f>
+        <v>500</v>
+      </c>
+      <c r="H22" s="7">
         <v>5000</v>
       </c>
+      <c r="I22" s="9">
+        <f>(C22*E22+D22*F22+(168-C22-D22)*G22)*365/7</f>
+        <v>8303750</v>
+      </c>
+      <c r="J22" s="9">
+        <f>D22*F22*365/7</f>
+        <v>3832500</v>
+      </c>
+      <c r="K22" s="10">
+        <f>I22/365/24/H22</f>
+        <v>0.18958333333333333</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" ht="34" customHeight="1">
+      <c r="A23" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B23" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C23" s="5">
+        <v>35</v>
+      </c>
+      <c r="D23" s="5">
+        <v>49</v>
+      </c>
+      <c r="E23" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="F23" s="6">
+        <v>0.05</v>
+      </c>
+      <c r="G23" s="6">
+        <v>0.2</v>
+      </c>
+      <c r="H23" s="7">
+        <v>3</v>
+      </c>
+      <c r="I23" s="9">
+        <f>(C23*E23+D23*F23+(168-C23-D23)*G23)*365/7</f>
+        <v>1916.25</v>
+      </c>
+      <c r="J23" s="9">
+        <f>D23*F23*365/7</f>
+        <v>127.75000000000001</v>
+      </c>
+      <c r="K23" s="10">
+        <f>I23/365/24/H23</f>
+        <v>7.2916666666666671E-2</v>
+      </c>
     </row>
   </sheetData>
+  <autoFilter ref="A4:K21">
+    <sortState ref="A5:K23">
+      <sortCondition ref="A4:A23"/>
+    </sortState>
+  </autoFilter>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>

</xml_diff>